<commit_message>
update mockup room configuration file
</commit_message>
<xml_diff>
--- a/role_permission_files/mockup_room_configuration_v0.9.xlsx
+++ b/role_permission_files/mockup_room_configuration_v0.9.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Product Management &amp; Market Research\Product Development\Platform\MockUpRoomConfiguration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ming.wong\git\rigi\sso_rws\role_permission_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="version" sheetId="2" r:id="rId1"/>
     <sheet name="AP" sheetId="3" r:id="rId2"/>
     <sheet name="SSO" sheetId="5" r:id="rId3"/>
-    <sheet name="Cage" sheetId="6" r:id="rId4"/>
+    <sheet name="CAGE" sheetId="6" r:id="rId4"/>
     <sheet name="GRMS" sheetId="7" r:id="rId5"/>
     <sheet name="SV" sheetId="8" r:id="rId6"/>
     <sheet name="SM" sheetId="10" r:id="rId7"/>

</xml_diff>